<commit_message>
V2.1 - Spreadsheet fetching
</commit_message>
<xml_diff>
--- a/Painting Record.xlsx
+++ b/Painting Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath-my.sharepoint.com/personal/francisco_lopez-marquez_2023_uni_strath_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopez\Desktop\V2.0 Javier_LeonhArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B6198B-5E77-48A4-BD2F-859F66FE2AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE4E6F32-D61D-458F-9B8C-5A3B66CBA60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="9766" windowHeight="12083" xr2:uid="{8FABD0BB-35D2-4746-8BF5-22ED6BD8493F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FABD0BB-35D2-4746-8BF5-22ED6BD8493F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -555,13 +555,19 @@
   </si>
   <si>
     <t>Tree-Revenants</t>
+  </si>
+  <si>
+    <t>Current Project</t>
+  </si>
+  <si>
+    <t>5x Tree-Revenants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,63 +604,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="22" formatCode="mmm\-yy"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -774,6 +723,63 @@
           <bgColor theme="8"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="22" formatCode="mmm\-yy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2693,7 +2699,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{61558924-6BAF-41CB-A458-0F8F58CE51F4}" name="Table2" displayName="Table2" ref="A1:F168" totalsRowShown="0">
   <autoFilter ref="A1:F168" xr:uid="{61558924-6BAF-41CB-A458-0F8F58CE51F4}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A1C8C315-1AF4-46A9-829B-F6F66670A080}" name="Date" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A1C8C315-1AF4-46A9-829B-F6F66670A080}" name="Date" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{5DD88343-1F7A-4E8C-82DC-76B842BC6326}" name="Project"/>
     <tableColumn id="3" xr3:uid="{67609590-421E-40D3-9386-469D330E5B1F}" name="Models"/>
     <tableColumn id="4" xr3:uid="{9FCCF59F-1639-4D57-AF65-D761F289622C}" name="Description"/>
@@ -2705,10 +2711,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FC8574FA-7BC0-4EFA-AA32-0A78DAD891B2}" name="Table3" displayName="Table3" ref="J1:J11" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FC8574FA-7BC0-4EFA-AA32-0A78DAD891B2}" name="Table3" displayName="Table3" ref="J1:J11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="J1:J11" xr:uid="{FC8574FA-7BC0-4EFA-AA32-0A78DAD891B2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{7B07971A-E433-4A37-8E69-8414A8DAFA6A}" name="Project List" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7B07971A-E433-4A37-8E69-8414A8DAFA6A}" name="Project List" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2721,6 +2727,16 @@
     <tableColumn id="1" xr3:uid="{55DB5F22-E9C6-43F4-91B3-C8775CAB6E79}" name="Total Painted">
       <calculatedColumnFormula>SUM(C2:C1020)</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE71C9D9-D413-42D0-B286-843925E7A779}" name="Table1" displayName="Table1" ref="H4:H5" totalsRowShown="0">
+  <autoFilter ref="H4:H5" xr:uid="{DE71C9D9-D413-42D0-B286-843925E7A779}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{285C54AE-A2BC-44AD-A7FA-881113AFB25A}" name="Current Project"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3046,22 +3062,22 @@
   <dimension ref="A1:J168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3087,7 +3103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>43405</v>
       </c>
@@ -3114,7 +3130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>43770</v>
       </c>
@@ -3137,7 +3153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>43435</v>
       </c>
@@ -3156,11 +3172,14 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
+      <c r="H4" t="s">
+        <v>173</v>
+      </c>
       <c r="J4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>43466</v>
       </c>
@@ -3179,11 +3198,14 @@
       <c r="F5" t="s">
         <v>11</v>
       </c>
+      <c r="H5" t="s">
+        <v>174</v>
+      </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>43466</v>
       </c>
@@ -3206,7 +3228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>43466</v>
       </c>
@@ -3229,7 +3251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>43497</v>
       </c>
@@ -3252,7 +3274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>43497</v>
       </c>
@@ -3275,7 +3297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>43525</v>
       </c>
@@ -3298,7 +3320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>43556</v>
       </c>
@@ -3321,7 +3343,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>43586</v>
       </c>
@@ -3341,7 +3363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>43586</v>
       </c>
@@ -3361,7 +3383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>43586</v>
       </c>
@@ -3381,7 +3403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>43586</v>
       </c>
@@ -3401,7 +3423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>43617</v>
       </c>
@@ -3421,7 +3443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>43617</v>
       </c>
@@ -3441,7 +3463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>43617</v>
       </c>
@@ -3461,7 +3483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>43617</v>
       </c>
@@ -3481,7 +3503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>43647</v>
       </c>
@@ -3501,7 +3523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>43647</v>
       </c>
@@ -3521,7 +3543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>43678</v>
       </c>
@@ -3541,7 +3563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>43678</v>
       </c>
@@ -3561,7 +3583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>43678</v>
       </c>
@@ -3581,7 +3603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>43678</v>
       </c>
@@ -3601,7 +3623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>43709</v>
       </c>
@@ -3621,7 +3643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>43709</v>
       </c>
@@ -3641,7 +3663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>43709</v>
       </c>
@@ -3661,7 +3683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>43739</v>
       </c>
@@ -3681,7 +3703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>43739</v>
       </c>
@@ -3701,7 +3723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>43739</v>
       </c>
@@ -3721,7 +3743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>43739</v>
       </c>
@@ -3741,7 +3763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>43739</v>
       </c>
@@ -3761,7 +3783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>43739</v>
       </c>
@@ -3781,7 +3803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>43739</v>
       </c>
@@ -3801,7 +3823,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>43739</v>
       </c>
@@ -3821,7 +3843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>43739</v>
       </c>
@@ -3841,7 +3863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>43770</v>
       </c>
@@ -3861,7 +3883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>43770</v>
       </c>
@@ -3881,7 +3903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>43770</v>
       </c>
@@ -3901,7 +3923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>43800</v>
       </c>
@@ -3921,7 +3943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>43831</v>
       </c>
@@ -3941,7 +3963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>43831</v>
       </c>
@@ -3961,7 +3983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43831</v>
       </c>
@@ -3981,7 +4003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43831</v>
       </c>
@@ -4001,7 +4023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>43831</v>
       </c>
@@ -4021,7 +4043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>43862</v>
       </c>
@@ -4041,7 +4063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>43862</v>
       </c>
@@ -4061,7 +4083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>43862</v>
       </c>
@@ -4081,7 +4103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>43862</v>
       </c>
@@ -4101,7 +4123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>43862</v>
       </c>
@@ -4121,7 +4143,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>43862</v>
       </c>
@@ -4141,7 +4163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>43862</v>
       </c>
@@ -4161,7 +4183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>43862</v>
       </c>
@@ -4181,7 +4203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>43862</v>
       </c>
@@ -4201,7 +4223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>43862</v>
       </c>
@@ -4221,7 +4243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>43862</v>
       </c>
@@ -4241,7 +4263,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>43862</v>
       </c>
@@ -4261,7 +4283,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>43862</v>
       </c>
@@ -4281,7 +4303,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>43891</v>
       </c>
@@ -4301,7 +4323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>43891</v>
       </c>
@@ -4321,7 +4343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>43891</v>
       </c>
@@ -4341,7 +4363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>43891</v>
       </c>
@@ -4361,7 +4383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>43891</v>
       </c>
@@ -4381,7 +4403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>43891</v>
       </c>
@@ -4401,7 +4423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>43922</v>
       </c>
@@ -4421,7 +4443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>43922</v>
       </c>
@@ -4441,7 +4463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>43922</v>
       </c>
@@ -4461,7 +4483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>43922</v>
       </c>
@@ -4481,7 +4503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>43922</v>
       </c>
@@ -4501,7 +4523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>43952</v>
       </c>
@@ -4521,7 +4543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>43952</v>
       </c>
@@ -4541,7 +4563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>43952</v>
       </c>
@@ -4561,7 +4583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>43952</v>
       </c>
@@ -4581,7 +4603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>43952</v>
       </c>
@@ -4601,7 +4623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>43952</v>
       </c>
@@ -4621,7 +4643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>43983</v>
       </c>
@@ -4641,7 +4663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>43983</v>
       </c>
@@ -4661,7 +4683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>43983</v>
       </c>
@@ -4681,7 +4703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>43983</v>
       </c>
@@ -4701,7 +4723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>43983</v>
       </c>
@@ -4721,7 +4743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>43983</v>
       </c>
@@ -4741,7 +4763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>44013</v>
       </c>
@@ -4749,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>44044</v>
       </c>
@@ -4769,7 +4791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>44044</v>
       </c>
@@ -4789,7 +4811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>44044</v>
       </c>
@@ -4809,7 +4831,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>44044</v>
       </c>
@@ -4829,7 +4851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>44044</v>
       </c>
@@ -4849,7 +4871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>44044</v>
       </c>
@@ -4869,7 +4891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>44044</v>
       </c>
@@ -4889,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>44075</v>
       </c>
@@ -4909,7 +4931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>44075</v>
       </c>
@@ -4929,7 +4951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>44075</v>
       </c>
@@ -4949,7 +4971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>44075</v>
       </c>
@@ -4969,7 +4991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>44075</v>
       </c>
@@ -4989,7 +5011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>44075</v>
       </c>
@@ -5009,7 +5031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>44075</v>
       </c>
@@ -5029,7 +5051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>44075</v>
       </c>
@@ -5049,7 +5071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>44075</v>
       </c>
@@ -5069,7 +5091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>44075</v>
       </c>
@@ -5089,7 +5111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>44075</v>
       </c>
@@ -5109,7 +5131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>44075</v>
       </c>
@@ -5129,7 +5151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>44105</v>
       </c>
@@ -5137,7 +5159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>44136</v>
       </c>
@@ -5145,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>44166</v>
       </c>
@@ -5153,7 +5175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>44197</v>
       </c>
@@ -5161,7 +5183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>44228</v>
       </c>
@@ -5169,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>44256</v>
       </c>
@@ -5189,7 +5211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>44287</v>
       </c>
@@ -5209,7 +5231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>44287</v>
       </c>
@@ -5229,7 +5251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>44287</v>
       </c>
@@ -5249,7 +5271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>44317</v>
       </c>
@@ -5269,7 +5291,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>44317</v>
       </c>
@@ -5289,7 +5311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>44317</v>
       </c>
@@ -5309,7 +5331,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>44348</v>
       </c>
@@ -5317,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>44378</v>
       </c>
@@ -5325,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>44409</v>
       </c>
@@ -5345,7 +5367,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>44409</v>
       </c>
@@ -5365,7 +5387,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>44409</v>
       </c>
@@ -5385,7 +5407,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>44409</v>
       </c>
@@ -5405,7 +5427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>44409</v>
       </c>
@@ -5425,7 +5447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>44409</v>
       </c>
@@ -5445,7 +5467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>44440</v>
       </c>
@@ -5465,7 +5487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>44470</v>
       </c>
@@ -5473,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>44501</v>
       </c>
@@ -5493,7 +5515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>44531</v>
       </c>
@@ -5513,7 +5535,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>44531</v>
       </c>
@@ -5533,7 +5555,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>44531</v>
       </c>
@@ -5553,7 +5575,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>44531</v>
       </c>
@@ -5573,7 +5595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>44562</v>
       </c>
@@ -5593,7 +5615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>44593</v>
       </c>
@@ -5613,7 +5635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>44593</v>
       </c>
@@ -5633,7 +5655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>44621</v>
       </c>
@@ -5653,7 +5675,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>44621</v>
       </c>
@@ -5673,7 +5695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>44621</v>
       </c>
@@ -5693,7 +5715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>44652</v>
       </c>
@@ -5713,7 +5735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>44682</v>
       </c>
@@ -5733,7 +5755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>44682</v>
       </c>
@@ -5753,7 +5775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>44682</v>
       </c>
@@ -5773,7 +5795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>44713</v>
       </c>
@@ -5793,7 +5815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>44713</v>
       </c>
@@ -5813,7 +5835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>44743</v>
       </c>
@@ -5833,7 +5855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>44774</v>
       </c>
@@ -5853,7 +5875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>44805</v>
       </c>
@@ -5873,7 +5895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>44835</v>
       </c>
@@ -5893,7 +5915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>44866</v>
       </c>
@@ -5913,7 +5935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>44896</v>
       </c>
@@ -5921,7 +5943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>44927</v>
       </c>
@@ -5941,7 +5963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>44927</v>
       </c>
@@ -5961,7 +5983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>44958</v>
       </c>
@@ -5981,7 +6003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>44986</v>
       </c>
@@ -6001,7 +6023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>44986</v>
       </c>
@@ -6021,7 +6043,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>45017</v>
       </c>
@@ -6029,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>45047</v>
       </c>
@@ -6037,7 +6059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>45078</v>
       </c>
@@ -6045,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>45108</v>
       </c>
@@ -6053,7 +6075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>45139</v>
       </c>
@@ -6061,7 +6083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>45170</v>
       </c>
@@ -6081,7 +6103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>45200</v>
       </c>
@@ -6089,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>45231</v>
       </c>
@@ -6097,7 +6119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>45261</v>
       </c>
@@ -6117,7 +6139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>45292</v>
       </c>
@@ -6125,7 +6147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>45323</v>
       </c>
@@ -6133,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>45352</v>
       </c>
@@ -6141,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>45383</v>
       </c>
@@ -6149,7 +6171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>45413</v>
       </c>
@@ -6169,7 +6191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>45474</v>
       </c>
@@ -6189,39 +6211,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J11 B2:B1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Sylvaneth Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Tunguska Warband"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"35mm Models"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"High Elves Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Lumineth Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Harlequins Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>"Ulthwé Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>"Slaves Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
       <formula>"Khorne Army"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
       <formula>"Practice"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6233,10 +6255,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V2.2.3 - Interface corrections
</commit_message>
<xml_diff>
--- a/Painting Record.xlsx
+++ b/Painting Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopez\Desktop\V2.2.1 Javier_LeonhArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A1B11F8-BAC1-4C4F-9FD1-1D9AFD6121DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19CC4C66-FE7E-455F-B857-29D4A438581C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FABD0BB-35D2-4746-8BF5-22ED6BD8493F}"/>
   </bookViews>
@@ -4184,7 +4184,7 @@
   <dimension ref="A1:J168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7521,7 +7521,7 @@
         <v>332</v>
       </c>
       <c r="D2">
-        <f>SUM(E2,G2,I2,K2,M2,O2)</f>
+        <f t="shared" ref="D2:D65" si="0">SUM(E2,G2,I2,K2,M2,O2)</f>
         <v>0</v>
       </c>
     </row>
@@ -7536,7 +7536,7 @@
         <v>336</v>
       </c>
       <c r="D3">
-        <f>SUM(E3,G3,I3,K3,M3,O3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7551,7 +7551,7 @@
         <v>276</v>
       </c>
       <c r="D4">
-        <f>SUM(E4,G4,I4,K4,M4,O4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4">
@@ -7572,7 +7572,7 @@
         <v>319</v>
       </c>
       <c r="D5">
-        <f>SUM(E5,G5,I5,K5,M5,O5)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E5">
@@ -7605,7 +7605,7 @@
         <v>276</v>
       </c>
       <c r="D6">
-        <f>SUM(E6,G6,I6,K6,M6,O6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G6">
@@ -7626,7 +7626,7 @@
         <v>330</v>
       </c>
       <c r="D7">
-        <f>SUM(E7,G7,I7,K7,M7,O7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7641,7 +7641,7 @@
         <v>297</v>
       </c>
       <c r="D8">
-        <f>SUM(E8,G8,I8,K8,M8,O8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M8">
@@ -7662,7 +7662,7 @@
         <v>276</v>
       </c>
       <c r="D9">
-        <f>SUM(E9,G9,I9,K9,M9,O9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7677,7 +7677,7 @@
         <v>297</v>
       </c>
       <c r="D10">
-        <f>SUM(E10,G10,I10,K10,M10,O10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G10">
@@ -7698,7 +7698,7 @@
         <v>244</v>
       </c>
       <c r="D11">
-        <f>SUM(E11,G11,I11,K11,M11,O11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7713,7 +7713,7 @@
         <v>332</v>
       </c>
       <c r="D12">
-        <f>SUM(E12,G12,I12,K12,M12,O12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7728,7 +7728,7 @@
         <v>336</v>
       </c>
       <c r="D13">
-        <f>SUM(E13,G13,I13,K13,M13,O13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7743,7 +7743,7 @@
         <v>336</v>
       </c>
       <c r="D14">
-        <f>SUM(E14,G14,I14,K14,M14,O14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7758,7 +7758,7 @@
         <v>332</v>
       </c>
       <c r="D15">
-        <f>SUM(E15,G15,I15,K15,M15,O15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H15">
@@ -7782,7 +7782,7 @@
         <v>312</v>
       </c>
       <c r="D16">
-        <f>SUM(E16,G16,I16,K16,M16,O16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K16">
@@ -7803,7 +7803,7 @@
         <v>269</v>
       </c>
       <c r="D17">
-        <f>SUM(E17,G17,I17,K17,M17,O17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7818,7 +7818,7 @@
         <v>269</v>
       </c>
       <c r="D18">
-        <f>SUM(E18,G18,I18,K18,M18,O18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O18">
@@ -7839,7 +7839,7 @@
         <v>244</v>
       </c>
       <c r="D19">
-        <f>SUM(E19,G19,I19,K19,M19,O19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7854,7 +7854,7 @@
         <v>269</v>
       </c>
       <c r="D20">
-        <f>SUM(E20,G20,I20,K20,M20,O20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7869,7 +7869,7 @@
         <v>297</v>
       </c>
       <c r="D21">
-        <f>SUM(E21,G21,I21,K21,M21,O21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K21">
@@ -7896,7 +7896,7 @@
         <v>276</v>
       </c>
       <c r="D22">
-        <f>SUM(E22,G22,I22,K22,M22,O22)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E22">
@@ -7920,7 +7920,7 @@
         <v>269</v>
       </c>
       <c r="D23">
-        <f>SUM(E23,G23,I23,K23,M23,O23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7935,7 +7935,7 @@
         <v>243</v>
       </c>
       <c r="D24">
-        <f>SUM(E24,G24,I24,K24,M24,O24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24">
@@ -7986,7 +7986,7 @@
         <v>243</v>
       </c>
       <c r="D25">
-        <f>SUM(E25,G25,I25,K25,M25,O25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25">
@@ -8037,7 +8037,7 @@
         <v>240</v>
       </c>
       <c r="D26">
-        <f>SUM(E26,G26,I26,K26,M26,O26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8052,7 +8052,7 @@
         <v>297</v>
       </c>
       <c r="D27">
-        <f>SUM(E27,G27,I27,K27,M27,O27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G27">
@@ -8073,7 +8073,7 @@
         <v>312</v>
       </c>
       <c r="D28">
-        <f>SUM(E28,G28,I28,K28,M28,O28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8088,7 +8088,7 @@
         <v>244</v>
       </c>
       <c r="D29">
-        <f>SUM(E29,G29,I29,K29,M29,O29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8103,7 +8103,7 @@
         <v>269</v>
       </c>
       <c r="D30">
-        <f>SUM(E30,G30,I30,K30,M30,O30)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M30">
@@ -8130,7 +8130,7 @@
         <v>332</v>
       </c>
       <c r="D31">
-        <f>SUM(E31,G31,I31,K31,M31,O31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M31">
@@ -8151,7 +8151,7 @@
         <v>269</v>
       </c>
       <c r="D32">
-        <f>SUM(E32,G32,I32,K32,M32,O32)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K32">
@@ -8178,7 +8178,7 @@
         <v>458</v>
       </c>
       <c r="D33">
-        <f>SUM(E33,G33,I33,K33,M33,O33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8193,7 +8193,7 @@
         <v>246</v>
       </c>
       <c r="D34">
-        <f>SUM(E34,G34,I34,K34,M34,O34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8208,7 +8208,7 @@
         <v>239</v>
       </c>
       <c r="D35">
-        <f>SUM(E35,G35,I35,K35,M35,O35)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8223,7 +8223,7 @@
         <v>239</v>
       </c>
       <c r="D36">
-        <f>SUM(E36,G36,I36,K36,M36,O36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8238,7 +8238,7 @@
         <v>332</v>
       </c>
       <c r="D37">
-        <f>SUM(E37,G37,I37,K37,M37,O37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8253,7 +8253,7 @@
         <v>312</v>
       </c>
       <c r="D38">
-        <f>SUM(E38,G38,I38,K38,M38,O38)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K38">
@@ -8274,7 +8274,7 @@
         <v>244</v>
       </c>
       <c r="D39">
-        <f>SUM(E39,G39,I39,K39,M39,O39)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8289,7 +8289,7 @@
         <v>269</v>
       </c>
       <c r="D40">
-        <f>SUM(E40,G40,I40,K40,M40,O40)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E40">
@@ -8310,7 +8310,7 @@
         <v>238</v>
       </c>
       <c r="D41">
-        <f>SUM(E41,G41,I41,K41,M41,O41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8325,7 +8325,7 @@
         <v>330</v>
       </c>
       <c r="D42">
-        <f>SUM(E42,G42,I42,K42,M42,O42)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8340,7 +8340,7 @@
         <v>458</v>
       </c>
       <c r="D43">
-        <f>SUM(E43,G43,I43,K43,M43,O43)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8355,7 +8355,7 @@
         <v>332</v>
       </c>
       <c r="D44">
-        <f>SUM(E44,G44,I44,K44,M44,O44)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8370,7 +8370,7 @@
         <v>276</v>
       </c>
       <c r="D45">
-        <f>SUM(E45,G45,I45,K45,M45,O45)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M45">
@@ -8388,7 +8388,7 @@
         <v>276</v>
       </c>
       <c r="D46">
-        <f>SUM(E46,G46,I46,K46,M46,O46)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K46">
@@ -8409,7 +8409,7 @@
         <v>332</v>
       </c>
       <c r="D47">
-        <f>SUM(E47,G47,I47,K47,M47,O47)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E47">
@@ -8430,7 +8430,7 @@
         <v>269</v>
       </c>
       <c r="D48">
-        <f>SUM(E48,G48,I48,K48,M48,O48)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8445,7 +8445,7 @@
         <v>330</v>
       </c>
       <c r="D49">
-        <f>SUM(E49,G49,I49,K49,M49,O49)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8460,7 +8460,7 @@
         <v>242</v>
       </c>
       <c r="D50">
-        <f>SUM(E50,G50,I50,K50,M50,O50)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G50">
@@ -8478,7 +8478,7 @@
         <v>336</v>
       </c>
       <c r="D51">
-        <f>SUM(E51,G51,I51,K51,M51,O51)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8493,7 +8493,7 @@
         <v>269</v>
       </c>
       <c r="D52">
-        <f>SUM(E52,G52,I52,K52,M52,O52)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8508,7 +8508,7 @@
         <v>336</v>
       </c>
       <c r="D53">
-        <f>SUM(E53,G53,I53,K53,M53,O53)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8523,7 +8523,7 @@
         <v>268</v>
       </c>
       <c r="D54">
-        <f>SUM(E54,G54,I54,K54,M54,O54)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8538,7 +8538,7 @@
         <v>269</v>
       </c>
       <c r="D55">
-        <f>SUM(E55,G55,I55,K55,M55,O55)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K55">
@@ -8559,7 +8559,7 @@
         <v>312</v>
       </c>
       <c r="D56">
-        <f>SUM(E56,G56,I56,K56,M56,O56)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K56">
@@ -8580,7 +8580,7 @@
         <v>297</v>
       </c>
       <c r="D57">
-        <f>SUM(E57,G57,I57,K57,M57,O57)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8595,7 +8595,7 @@
         <v>288</v>
       </c>
       <c r="D58">
-        <f>SUM(E58,G58,I58,K58,M58,O58)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K58">
@@ -8616,7 +8616,7 @@
         <v>244</v>
       </c>
       <c r="D59">
-        <f>SUM(E59,G59,I59,K59,M59,O59)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8631,7 +8631,7 @@
         <v>297</v>
       </c>
       <c r="D60">
-        <f>SUM(E60,G60,I60,K60,M60,O60)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8646,7 +8646,7 @@
         <v>330</v>
       </c>
       <c r="D61">
-        <f>SUM(E61,G61,I61,K61,M61,O61)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8661,7 +8661,7 @@
         <v>336</v>
       </c>
       <c r="D62">
-        <f>SUM(E62,G62,I62,K62,M62,O62)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K62">
@@ -8682,7 +8682,7 @@
         <v>241</v>
       </c>
       <c r="D63">
-        <f>SUM(E63,G63,I63,K63,M63,O63)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8697,7 +8697,7 @@
         <v>319</v>
       </c>
       <c r="D64">
-        <f>SUM(E64,G64,I64,K64,M64,O64)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E64">
@@ -8730,7 +8730,7 @@
         <v>312</v>
       </c>
       <c r="D65">
-        <f>SUM(E65,G65,I65,K65,M65,O65)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K65">
@@ -8751,7 +8751,7 @@
         <v>269</v>
       </c>
       <c r="D66">
-        <f>SUM(E66,G66,I66,K66,M66,O66)</f>
+        <f t="shared" ref="D66:D129" si="1">SUM(E66,G66,I66,K66,M66,O66)</f>
         <v>0</v>
       </c>
     </row>
@@ -8766,7 +8766,7 @@
         <v>336</v>
       </c>
       <c r="D67">
-        <f>SUM(E67,G67,I67,K67,M67,O67)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8781,7 +8781,7 @@
         <v>312</v>
       </c>
       <c r="D68">
-        <f>SUM(E68,G68,I68,K68,M68,O68)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K68">
@@ -8802,7 +8802,7 @@
         <v>336</v>
       </c>
       <c r="D69">
-        <f>SUM(E69,G69,I69,K69,M69,O69)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8817,7 +8817,7 @@
         <v>238</v>
       </c>
       <c r="D70">
-        <f>SUM(E70,G70,I70,K70,M70,O70)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8832,7 +8832,7 @@
         <v>336</v>
       </c>
       <c r="D71">
-        <f>SUM(E71,G71,I71,K71,M71,O71)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8847,7 +8847,7 @@
         <v>244</v>
       </c>
       <c r="D72">
-        <f>SUM(E72,G72,I72,K72,M72,O72)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8862,7 +8862,7 @@
         <v>336</v>
       </c>
       <c r="D73">
-        <f>SUM(E73,G73,I73,K73,M73,O73)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8877,7 +8877,7 @@
         <v>336</v>
       </c>
       <c r="D74">
-        <f>SUM(E74,G74,I74,K74,M74,O74)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8892,7 +8892,7 @@
         <v>297</v>
       </c>
       <c r="D75">
-        <f>SUM(E75,G75,I75,K75,M75,O75)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8907,7 +8907,7 @@
         <v>332</v>
       </c>
       <c r="D76">
-        <f>SUM(E76,G76,I76,K76,M76,O76)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8922,7 +8922,7 @@
         <v>269</v>
       </c>
       <c r="D77">
-        <f>SUM(E77,G77,I77,K77,M77,O77)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8937,7 +8937,7 @@
         <v>312</v>
       </c>
       <c r="D78">
-        <f>SUM(E78,G78,I78,K78,M78,O78)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8952,7 +8952,7 @@
         <v>268</v>
       </c>
       <c r="D79">
-        <f>SUM(E79,G79,I79,K79,M79,O79)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8967,7 +8967,7 @@
         <v>312</v>
       </c>
       <c r="D80">
-        <f>SUM(E80,G80,I80,K80,M80,O80)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8982,7 +8982,7 @@
         <v>239</v>
       </c>
       <c r="D81">
-        <f>SUM(E81,G81,I81,K81,M81,O81)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
         <v>297</v>
       </c>
       <c r="D82">
-        <f>SUM(E82,G82,I82,K82,M82,O82)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K82">
@@ -9018,7 +9018,7 @@
         <v>297</v>
       </c>
       <c r="D83">
-        <f>SUM(E83,G83,I83,K83,M83,O83)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O83">
@@ -9039,7 +9039,7 @@
         <v>276</v>
       </c>
       <c r="D84">
-        <f>SUM(E84,G84,I84,K84,M84,O84)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M84">
@@ -9057,7 +9057,7 @@
         <v>312</v>
       </c>
       <c r="D85">
-        <f>SUM(E85,G85,I85,K85,M85,O85)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M85">
@@ -9078,7 +9078,7 @@
         <v>297</v>
       </c>
       <c r="D86">
-        <f>SUM(E86,G86,I86,K86,M86,O86)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9093,7 +9093,7 @@
         <v>269</v>
       </c>
       <c r="D87">
-        <f>SUM(E87,G87,I87,K87,M87,O87)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9108,7 +9108,7 @@
         <v>332</v>
       </c>
       <c r="D88">
-        <f>SUM(E88,G88,I88,K88,M88,O88)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M88">
@@ -9129,7 +9129,7 @@
         <v>297</v>
       </c>
       <c r="D89">
-        <f>SUM(E89,G89,I89,K89,M89,O89)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E89">
@@ -9162,7 +9162,7 @@
         <v>238</v>
       </c>
       <c r="D90">
-        <f>SUM(E90,G90,I90,K90,M90,O90)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9177,7 +9177,7 @@
         <v>312</v>
       </c>
       <c r="D91">
-        <f>SUM(E91,G91,I91,K91,M91,O91)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M91">
@@ -9198,7 +9198,7 @@
         <v>276</v>
       </c>
       <c r="D92">
-        <f>SUM(E92,G92,I92,K92,M92,O92)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9213,7 +9213,7 @@
         <v>276</v>
       </c>
       <c r="D93">
-        <f>SUM(E93,G93,I93,K93,M93,O93)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9228,7 +9228,7 @@
         <v>292</v>
       </c>
       <c r="D94">
-        <f>SUM(E94,G94,I94,K94,M94,O94)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9243,7 +9243,7 @@
         <v>292</v>
       </c>
       <c r="D95">
-        <f>SUM(E95,G95,I95,K95,M95,O95)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9258,7 +9258,7 @@
         <v>292</v>
       </c>
       <c r="D96">
-        <f>SUM(E96,G96,I96,K96,M96,O96)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9273,7 +9273,7 @@
         <v>292</v>
       </c>
       <c r="D97">
-        <f>SUM(E97,G97,I97,K97,M97,O97)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K97">
@@ -9294,7 +9294,7 @@
         <v>292</v>
       </c>
       <c r="D98">
-        <f>SUM(E98,G98,I98,K98,M98,O98)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9309,7 +9309,7 @@
         <v>292</v>
       </c>
       <c r="D99">
-        <f>SUM(E99,G99,I99,K99,M99,O99)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G99">
@@ -9333,7 +9333,7 @@
         <v>292</v>
       </c>
       <c r="D100">
-        <f>SUM(E100,G100,I100,K100,M100,O100)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E100">
@@ -9366,7 +9366,7 @@
         <v>330</v>
       </c>
       <c r="D101">
-        <f>SUM(E101,G101,I101,K101,M101,O101)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9381,7 +9381,7 @@
         <v>288</v>
       </c>
       <c r="D102">
-        <f>SUM(E102,G102,I102,K102,M102,O102)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E102">
@@ -9402,7 +9402,7 @@
         <v>297</v>
       </c>
       <c r="D103">
-        <f>SUM(E103,G103,I103,K103,M103,O103)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9417,7 +9417,7 @@
         <v>269</v>
       </c>
       <c r="D104">
-        <f>SUM(E104,G104,I104,K104,M104,O104)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E104">
@@ -9468,7 +9468,7 @@
         <v>332</v>
       </c>
       <c r="D105">
-        <f>SUM(E105,G105,I105,K105,M105,O105)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9483,7 +9483,7 @@
         <v>238</v>
       </c>
       <c r="D106">
-        <f>SUM(E106,G106,I106,K106,M106,O106)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9498,7 +9498,7 @@
         <v>269</v>
       </c>
       <c r="D107">
-        <f>SUM(E107,G107,I107,K107,M107,O107)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9513,7 +9513,7 @@
         <v>276</v>
       </c>
       <c r="D108">
-        <f>SUM(E108,G108,I108,K108,M108,O108)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9528,7 +9528,7 @@
         <v>297</v>
       </c>
       <c r="D109">
-        <f>SUM(E109,G109,I109,K109,M109,O109)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="G109">
@@ -9555,7 +9555,7 @@
         <v>332</v>
       </c>
       <c r="D110">
-        <f>SUM(E110,G110,I110,K110,M110,O110)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M110">
@@ -9576,7 +9576,7 @@
         <v>336</v>
       </c>
       <c r="D111">
-        <f>SUM(E111,G111,I111,K111,M111,O111)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9591,7 +9591,7 @@
         <v>336</v>
       </c>
       <c r="D112">
-        <f>SUM(E112,G112,I112,K112,M112,O112)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9606,7 +9606,7 @@
         <v>312</v>
       </c>
       <c r="D113">
-        <f>SUM(E113,G113,I113,K113,M113,O113)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K113">
@@ -9627,7 +9627,7 @@
         <v>332</v>
       </c>
       <c r="D114">
-        <f>SUM(E114,G114,I114,K114,M114,O114)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9642,7 +9642,7 @@
         <v>239</v>
       </c>
       <c r="D115">
-        <f>SUM(E115,G115,I115,K115,M115,O115)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9657,7 +9657,7 @@
         <v>408</v>
       </c>
       <c r="D116">
-        <f>SUM(E116,G116,I116,K116,M116,O116)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E116">
@@ -9708,7 +9708,7 @@
         <v>297</v>
       </c>
       <c r="D117">
-        <f>SUM(E117,G117,I117,K117,M117,O117)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E117">
@@ -9759,7 +9759,7 @@
         <v>297</v>
       </c>
       <c r="D118">
-        <f>SUM(E118,G118,I118,K118,M118,O118)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E118">
@@ -9810,7 +9810,7 @@
         <v>297</v>
       </c>
       <c r="D119">
-        <f>SUM(E119,G119,I119,K119,M119,O119)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M119">
@@ -9831,7 +9831,7 @@
         <v>269</v>
       </c>
       <c r="D120">
-        <f>SUM(E120,G120,I120,K120,M120,O120)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9846,7 +9846,7 @@
         <v>297</v>
       </c>
       <c r="D121">
-        <f>SUM(E121,G121,I121,K121,M121,O121)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M121">
@@ -9867,7 +9867,7 @@
         <v>297</v>
       </c>
       <c r="D122">
-        <f>SUM(E122,G122,I122,K122,M122,O122)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9882,7 +9882,7 @@
         <v>297</v>
       </c>
       <c r="D123">
-        <f>SUM(E123,G123,I123,K123,M123,O123)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K123">
@@ -9903,7 +9903,7 @@
         <v>332</v>
       </c>
       <c r="D124">
-        <f>SUM(E124,G124,I124,K124,M124,O124)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9918,7 +9918,7 @@
         <v>458</v>
       </c>
       <c r="D125">
-        <f>SUM(E125,G125,I125,K125,M125,O125)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9933,7 +9933,7 @@
         <v>330</v>
       </c>
       <c r="D126">
-        <f>SUM(E126,G126,I126,K126,M126,O126)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9948,7 +9948,7 @@
         <v>332</v>
       </c>
       <c r="D127">
-        <f>SUM(E127,G127,I127,K127,M127,O127)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9963,7 +9963,7 @@
         <v>269</v>
       </c>
       <c r="D128">
-        <f>SUM(E128,G128,I128,K128,M128,O128)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K128">
@@ -9984,7 +9984,7 @@
         <v>244</v>
       </c>
       <c r="D129">
-        <f>SUM(E129,G129,I129,K129,M129,O129)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9999,7 +9999,7 @@
         <v>312</v>
       </c>
       <c r="D130">
-        <f>SUM(E130,G130,I130,K130,M130,O130)</f>
+        <f t="shared" ref="D130:D193" si="2">SUM(E130,G130,I130,K130,M130,O130)</f>
         <v>1</v>
       </c>
       <c r="K130">
@@ -10020,7 +10020,7 @@
         <v>336</v>
       </c>
       <c r="D131">
-        <f>SUM(E131,G131,I131,K131,M131,O131)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10035,7 +10035,7 @@
         <v>332</v>
       </c>
       <c r="D132">
-        <f>SUM(E132,G132,I132,K132,M132,O132)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10050,7 +10050,7 @@
         <v>238</v>
       </c>
       <c r="D133">
-        <f>SUM(E133,G133,I133,K133,M133,O133)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10065,7 +10065,7 @@
         <v>332</v>
       </c>
       <c r="D134">
-        <f>SUM(E134,G134,I134,K134,M134,O134)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10080,7 +10080,7 @@
         <v>288</v>
       </c>
       <c r="D135">
-        <f>SUM(E135,G135,I135,K135,M135,O135)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E135">
@@ -10101,7 +10101,7 @@
         <v>244</v>
       </c>
       <c r="D136">
-        <f>SUM(E136,G136,I136,K136,M136,O136)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10116,7 +10116,7 @@
         <v>244</v>
       </c>
       <c r="D137">
-        <f>SUM(E137,G137,I137,K137,M137,O137)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10131,7 +10131,7 @@
         <v>244</v>
       </c>
       <c r="D138">
-        <f>SUM(E138,G138,I138,K138,M138,O138)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10146,7 +10146,7 @@
         <v>244</v>
       </c>
       <c r="D139">
-        <f>SUM(E139,G139,I139,K139,M139,O139)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10161,7 +10161,7 @@
         <v>244</v>
       </c>
       <c r="D140">
-        <f>SUM(E140,G140,I140,K140,M140,O140)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G140">
@@ -10182,7 +10182,7 @@
         <v>244</v>
       </c>
       <c r="D141">
-        <f>SUM(E141,G141,I141,K141,M141,O141)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10197,7 +10197,7 @@
         <v>276</v>
       </c>
       <c r="D142">
-        <f>SUM(E142,G142,I142,K142,M142,O142)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10212,7 +10212,7 @@
         <v>312</v>
       </c>
       <c r="D143">
-        <f>SUM(E143,G143,I143,K143,M143,O143)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M143">
@@ -10233,7 +10233,7 @@
         <v>244</v>
       </c>
       <c r="D144">
-        <f>SUM(E144,G144,I144,K144,M144,O144)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10248,7 +10248,7 @@
         <v>458</v>
       </c>
       <c r="D145">
-        <f>SUM(E145,G145,I145,K145,M145,O145)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10263,7 +10263,7 @@
         <v>330</v>
       </c>
       <c r="D146">
-        <f>SUM(E146,G146,I146,K146,M146,O146)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K146">
@@ -10284,7 +10284,7 @@
         <v>330</v>
       </c>
       <c r="D147">
-        <f>SUM(E147,G147,I147,K147,M147,O147)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K147">
@@ -10305,7 +10305,7 @@
         <v>330</v>
       </c>
       <c r="D148">
-        <f>SUM(E148,G148,I148,K148,M148,O148)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K148">
@@ -10326,7 +10326,7 @@
         <v>330</v>
       </c>
       <c r="D149">
-        <f>SUM(E149,G149,I149,K149,M149,O149)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10341,7 +10341,7 @@
         <v>269</v>
       </c>
       <c r="D150">
-        <f>SUM(E150,G150,I150,K150,M150,O150)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10356,7 +10356,7 @@
         <v>269</v>
       </c>
       <c r="D151">
-        <f>SUM(E151,G151,I151,K151,M151,O151)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10371,7 +10371,7 @@
         <v>336</v>
       </c>
       <c r="D152">
-        <f>SUM(E152,G152,I152,K152,M152,O152)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10386,7 +10386,7 @@
         <v>332</v>
       </c>
       <c r="D153">
-        <f>SUM(E153,G153,I153,K153,M153,O153)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10401,7 +10401,7 @@
         <v>458</v>
       </c>
       <c r="D154">
-        <f>SUM(E154,G154,I154,K154,M154,O154)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10416,7 +10416,7 @@
         <v>458</v>
       </c>
       <c r="D155">
-        <f>SUM(E155,G155,I155,K155,M155,O155)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10431,7 +10431,7 @@
         <v>458</v>
       </c>
       <c r="D156">
-        <f>SUM(E156,G156,I156,K156,M156,O156)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10446,7 +10446,7 @@
         <v>244</v>
       </c>
       <c r="D157">
-        <f>SUM(E157,G157,I157,K157,M157,O157)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10461,7 +10461,7 @@
         <v>336</v>
       </c>
       <c r="D158">
-        <f>SUM(E158,G158,I158,K158,M158,O158)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10476,7 +10476,7 @@
         <v>297</v>
       </c>
       <c r="D159">
-        <f>SUM(E159,G159,I159,K159,M159,O159)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10491,7 +10491,7 @@
         <v>269</v>
       </c>
       <c r="D160">
-        <f>SUM(E160,G160,I160,K160,M160,O160)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10506,7 +10506,7 @@
         <v>297</v>
       </c>
       <c r="D161">
-        <f>SUM(E161,G161,I161,K161,M161,O161)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10521,7 +10521,7 @@
         <v>330</v>
       </c>
       <c r="D162">
-        <f>SUM(E162,G162,I162,K162,M162,O162)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10536,7 +10536,7 @@
         <v>297</v>
       </c>
       <c r="D163">
-        <f>SUM(E163,G163,I163,K163,M163,O163)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10551,7 +10551,7 @@
         <v>332</v>
       </c>
       <c r="D164">
-        <f>SUM(E164,G164,I164,K164,M164,O164)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10566,7 +10566,7 @@
         <v>276</v>
       </c>
       <c r="D165">
-        <f>SUM(E165,G165,I165,K165,M165,O165)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E165">
@@ -10593,7 +10593,7 @@
         <v>458</v>
       </c>
       <c r="D166">
-        <f>SUM(E166,G166,I166,K166,M166,O166)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10608,7 +10608,7 @@
         <v>242</v>
       </c>
       <c r="D167">
-        <f>SUM(E167,G167,I167,K167,M167,O167)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E167">
@@ -10641,7 +10641,7 @@
         <v>458</v>
       </c>
       <c r="D168">
-        <f>SUM(E168,G168,I168,K168,M168,O168)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10656,7 +10656,7 @@
         <v>297</v>
       </c>
       <c r="D169">
-        <f>SUM(E169,G169,I169,K169,M169,O169)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M169">
@@ -10677,7 +10677,7 @@
         <v>332</v>
       </c>
       <c r="D170">
-        <f>SUM(E170,G170,I170,K170,M170,O170)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10692,7 +10692,7 @@
         <v>330</v>
       </c>
       <c r="D171">
-        <f>SUM(E171,G171,I171,K171,M171,O171)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10707,7 +10707,7 @@
         <v>297</v>
       </c>
       <c r="D172">
-        <f>SUM(E172,G172,I172,K172,M172,O172)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O172">
@@ -10728,7 +10728,7 @@
         <v>239</v>
       </c>
       <c r="D173">
-        <f>SUM(E173,G173,I173,K173,M173,O173)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10743,7 +10743,7 @@
         <v>297</v>
       </c>
       <c r="D174">
-        <f>SUM(E174,G174,I174,K174,M174,O174)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M174">
@@ -10764,7 +10764,7 @@
         <v>312</v>
       </c>
       <c r="D175">
-        <f>SUM(E175,G175,I175,K175,M175,O175)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M175">
@@ -10785,7 +10785,7 @@
         <v>268</v>
       </c>
       <c r="D176">
-        <f>SUM(E176,G176,I176,K176,M176,O176)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10800,7 +10800,7 @@
         <v>332</v>
       </c>
       <c r="D177">
-        <f>SUM(E177,G177,I177,K177,M177,O177)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10815,7 +10815,7 @@
         <v>312</v>
       </c>
       <c r="D178">
-        <f>SUM(E178,G178,I178,K178,M178,O178)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M178">
@@ -10836,7 +10836,7 @@
         <v>297</v>
       </c>
       <c r="D179">
-        <f>SUM(E179,G179,I179,K179,M179,O179)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E179">
@@ -10863,7 +10863,7 @@
         <v>239</v>
       </c>
       <c r="D180">
-        <f>SUM(E180,G180,I180,K180,M180,O180)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10878,7 +10878,7 @@
         <v>276</v>
       </c>
       <c r="D181">
-        <f>SUM(E181,G181,I181,K181,M181,O181)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
         <v>269</v>
       </c>
       <c r="D182">
-        <f>SUM(E182,G182,I182,K182,M182,O182)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K182">
@@ -10914,7 +10914,7 @@
         <v>276</v>
       </c>
       <c r="D183">
-        <f>SUM(E183,G183,I183,K183,M183,O183)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10929,7 +10929,7 @@
         <v>336</v>
       </c>
       <c r="D184">
-        <f>SUM(E184,G184,I184,K184,M184,O184)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10944,7 +10944,7 @@
         <v>332</v>
       </c>
       <c r="D185">
-        <f>SUM(E185,G185,I185,K185,M185,O185)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K185">
@@ -10965,7 +10965,7 @@
         <v>269</v>
       </c>
       <c r="D186">
-        <f>SUM(E186,G186,I186,K186,M186,O186)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K186">
@@ -10986,7 +10986,7 @@
         <v>312</v>
       </c>
       <c r="D187">
-        <f>SUM(E187,G187,I187,K187,M187,O187)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M187">
@@ -11007,7 +11007,7 @@
         <v>238</v>
       </c>
       <c r="D188">
-        <f>SUM(E188,G188,I188,K188,M188,O188)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11022,7 +11022,7 @@
         <v>269</v>
       </c>
       <c r="D189">
-        <f>SUM(E189,G189,I189,K189,M189,O189)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11037,7 +11037,7 @@
         <v>269</v>
       </c>
       <c r="D190">
-        <f>SUM(E190,G190,I190,K190,M190,O190)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11052,7 +11052,7 @@
         <v>336</v>
       </c>
       <c r="D191">
-        <f>SUM(E191,G191,I191,K191,M191,O191)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11067,7 +11067,7 @@
         <v>336</v>
       </c>
       <c r="D192">
-        <f>SUM(E192,G192,I192,K192,M192,O192)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11082,7 +11082,7 @@
         <v>297</v>
       </c>
       <c r="D193">
-        <f>SUM(E193,G193,I193,K193,M193,O193)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E193">
@@ -11133,7 +11133,7 @@
         <v>332</v>
       </c>
       <c r="D194">
-        <f>SUM(E194,G194,I194,K194,M194,O194)</f>
+        <f t="shared" ref="D194:D257" si="3">SUM(E194,G194,I194,K194,M194,O194)</f>
         <v>0</v>
       </c>
     </row>
@@ -11148,7 +11148,7 @@
         <v>332</v>
       </c>
       <c r="D195">
-        <f>SUM(E195,G195,I195,K195,M195,O195)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11163,7 +11163,7 @@
         <v>336</v>
       </c>
       <c r="D196">
-        <f>SUM(E196,G196,I196,K196,M196,O196)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11178,7 +11178,7 @@
         <v>458</v>
       </c>
       <c r="D197">
-        <f>SUM(E197,G197,I197,K197,M197,O197)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11193,7 +11193,7 @@
         <v>244</v>
       </c>
       <c r="D198">
-        <f>SUM(E198,G198,I198,K198,M198,O198)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11208,7 +11208,7 @@
         <v>330</v>
       </c>
       <c r="D199">
-        <f>SUM(E199,G199,I199,K199,M199,O199)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11223,7 +11223,7 @@
         <v>312</v>
       </c>
       <c r="D200">
-        <f>SUM(E200,G200,I200,K200,M200,O200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K200">
@@ -11244,7 +11244,7 @@
         <v>244</v>
       </c>
       <c r="D201">
-        <f>SUM(E201,G201,I201,K201,M201,O201)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11259,7 +11259,7 @@
         <v>336</v>
       </c>
       <c r="D202">
-        <f>SUM(E202,G202,I202,K202,M202,O202)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11274,7 +11274,7 @@
         <v>244</v>
       </c>
       <c r="D203">
-        <f>SUM(E203,G203,I203,K203,M203,O203)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11289,7 +11289,7 @@
         <v>288</v>
       </c>
       <c r="D204">
-        <f>SUM(E204,G204,I204,K204,M204,O204)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G204">
@@ -11310,7 +11310,7 @@
         <v>336</v>
       </c>
       <c r="D205">
-        <f>SUM(E205,G205,I205,K205,M205,O205)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M205">
@@ -11331,7 +11331,7 @@
         <v>330</v>
       </c>
       <c r="D206">
-        <f>SUM(E206,G206,I206,K206,M206,O206)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11346,7 +11346,7 @@
         <v>244</v>
       </c>
       <c r="D207">
-        <f>SUM(E207,G207,I207,K207,M207,O207)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11361,7 +11361,7 @@
         <v>336</v>
       </c>
       <c r="D208">
-        <f>SUM(E208,G208,I208,K208,M208,O208)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O208">
@@ -11382,7 +11382,7 @@
         <v>288</v>
       </c>
       <c r="D209">
-        <f>SUM(E209,G209,I209,K209,M209,O209)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K209">
@@ -11403,7 +11403,7 @@
         <v>297</v>
       </c>
       <c r="D210">
-        <f>SUM(E210,G210,I210,K210,M210,O210)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K210">
@@ -11424,7 +11424,7 @@
         <v>458</v>
       </c>
       <c r="D211">
-        <f>SUM(E211,G211,I211,K211,M211,O211)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11439,7 +11439,7 @@
         <v>244</v>
       </c>
       <c r="D212">
-        <f>SUM(E212,G212,I212,K212,M212,O212)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11454,7 +11454,7 @@
         <v>297</v>
       </c>
       <c r="D213">
-        <f>SUM(E213,G213,I213,K213,M213,O213)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K213">
@@ -11475,7 +11475,7 @@
         <v>276</v>
       </c>
       <c r="D214">
-        <f>SUM(E214,G214,I214,K214,M214,O214)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11490,7 +11490,7 @@
         <v>312</v>
       </c>
       <c r="D215">
-        <f>SUM(E215,G215,I215,K215,M215,O215)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K215">
@@ -11511,7 +11511,7 @@
         <v>458</v>
       </c>
       <c r="D216">
-        <f>SUM(E216,G216,I216,K216,M216,O216)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11526,7 +11526,7 @@
         <v>288</v>
       </c>
       <c r="D217">
-        <f>SUM(E217,G217,I217,K217,M217,O217)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E217">
@@ -11553,7 +11553,7 @@
         <v>336</v>
       </c>
       <c r="D218">
-        <f>SUM(E218,G218,I218,K218,M218,O218)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11568,7 +11568,7 @@
         <v>297</v>
       </c>
       <c r="D219">
-        <f>SUM(E219,G219,I219,K219,M219,O219)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E219">
@@ -11601,7 +11601,7 @@
         <v>244</v>
       </c>
       <c r="D220">
-        <f>SUM(E220,G220,I220,K220,M220,O220)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11616,7 +11616,7 @@
         <v>332</v>
       </c>
       <c r="D221">
-        <f>SUM(E221,G221,I221,K221,M221,O221)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O221">
@@ -11637,7 +11637,7 @@
         <v>332</v>
       </c>
       <c r="D222">
-        <f>SUM(E222,G222,I222,K222,M222,O222)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11652,7 +11652,7 @@
         <v>244</v>
       </c>
       <c r="D223">
-        <f>SUM(E223,G223,I223,K223,M223,O223)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11667,7 +11667,7 @@
         <v>458</v>
       </c>
       <c r="D224">
-        <f>SUM(E224,G224,I224,K224,M224,O224)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11682,7 +11682,7 @@
         <v>336</v>
       </c>
       <c r="D225">
-        <f>SUM(E225,G225,I225,K225,M225,O225)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11697,7 +11697,7 @@
         <v>332</v>
       </c>
       <c r="D226">
-        <f>SUM(E226,G226,I226,K226,M226,O226)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O226">

</xml_diff>

<commit_message>
v3.1 - New title format
</commit_message>
<xml_diff>
--- a/Painting Record.xlsx
+++ b/Painting Record.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopez\Desktop\V2.6 Javier_LeonhArt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopez\Desktop\V3.0 Javier_LeonhArt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB62A6D-77ED-43E0-B8FC-A66C2FB73BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93DA299-C21B-42D3-991D-89BF8A0B77F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" activeTab="1" xr2:uid="{8FABD0BB-35D2-4746-8BF5-22ED6BD8493F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FABD0BB-35D2-4746-8BF5-22ED6BD8493F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1534,9 +1534,6 @@
     <t>Wings</t>
   </si>
   <si>
-    <t>On Break</t>
-  </si>
-  <si>
     <t>Ynnari Warlock</t>
   </si>
   <si>
@@ -1553,6 +1550,9 @@
   </si>
   <si>
     <t>Gems Main</t>
+  </si>
+  <si>
+    <t>5x Gossamid Archers</t>
   </si>
 </sst>
 </file>
@@ -4279,8 +4279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F725C0D8-4E5E-44F7-BED9-972635B5DB06}">
   <dimension ref="A1:J172"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4417,7 +4417,7 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -7529,7 +7529,7 @@
         <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E171" t="s">
         <v>43</v>
@@ -7597,7 +7597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD12CC97-8595-4312-A700-76C39152E1F0}">
   <dimension ref="A1:P236"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="108" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7682,7 +7682,7 @@
         <v>243</v>
       </c>
       <c r="D2">
-        <f>SUM(E2,G2,I2,K2,M2,O2)</f>
+        <f t="shared" ref="D2:D65" si="0">SUM(E2,G2,I2,K2,M2,O2)</f>
         <v>0</v>
       </c>
       <c r="E2">
@@ -7733,7 +7733,7 @@
         <v>296</v>
       </c>
       <c r="D3">
-        <f>SUM(E3,G3,I3,K3,M3,O3)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E3">
@@ -7772,7 +7772,7 @@
         <v>318</v>
       </c>
       <c r="D4">
-        <f>SUM(E4,G4,I4,K4,M4,O4)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E4">
@@ -7805,7 +7805,7 @@
         <v>318</v>
       </c>
       <c r="D5">
-        <f>SUM(E5,G5,I5,K5,M5,O5)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E5">
@@ -7838,7 +7838,7 @@
         <v>296</v>
       </c>
       <c r="D6">
-        <f>SUM(E6,G6,I6,K6,M6,O6)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E6">
@@ -7871,20 +7871,20 @@
         <v>455</v>
       </c>
       <c r="D7">
-        <f>SUM(E7,G7,I7,K7,M7,O7)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -7904,7 +7904,7 @@
         <v>241</v>
       </c>
       <c r="D8">
-        <f>SUM(E8,G8,I8,K8,M8,O8)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E8">
@@ -7937,7 +7937,7 @@
         <v>291</v>
       </c>
       <c r="D9">
-        <f>SUM(E9,G9,I9,K9,M9,O9)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E9">
@@ -7970,26 +7970,26 @@
         <v>291</v>
       </c>
       <c r="D10">
-        <f>SUM(E10,G10,I10,K10,M10,O10)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
@@ -8003,7 +8003,7 @@
         <v>287</v>
       </c>
       <c r="D11">
-        <f>SUM(E11,G11,I11,K11,M11,O11)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E11">
@@ -8036,7 +8036,7 @@
         <v>296</v>
       </c>
       <c r="D12">
-        <f>SUM(E12,G12,I12,K12,M12,O12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G12">
@@ -8063,7 +8063,7 @@
         <v>296</v>
       </c>
       <c r="D13">
-        <f>SUM(E13,G13,I13,K13,M13,O13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G13">
@@ -8090,7 +8090,7 @@
         <v>296</v>
       </c>
       <c r="D14">
-        <f>SUM(E14,G14,I14,K14,M14,O14)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K14">
@@ -8117,7 +8117,7 @@
         <v>296</v>
       </c>
       <c r="D15">
-        <f>SUM(E15,G15,I15,K15,M15,O15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K15">
@@ -8144,7 +8144,7 @@
         <v>296</v>
       </c>
       <c r="D16">
-        <f>SUM(E16,G16,I16,K16,M16,O16)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K16">
@@ -8171,7 +8171,7 @@
         <v>296</v>
       </c>
       <c r="D17">
-        <f>SUM(E17,G17,I17,K17,M17,O17)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E17">
@@ -8198,7 +8198,7 @@
         <v>296</v>
       </c>
       <c r="D18">
-        <f>SUM(E18,G18,I18,K18,M18,O18)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G18">
@@ -8225,7 +8225,7 @@
         <v>275</v>
       </c>
       <c r="D19">
-        <f>SUM(E19,G19,I19,K19,M19,O19)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E19">
@@ -8249,7 +8249,7 @@
         <v>275</v>
       </c>
       <c r="D20">
-        <f>SUM(E20,G20,I20,K20,M20,O20)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K20">
@@ -8273,7 +8273,7 @@
         <v>331</v>
       </c>
       <c r="D21">
-        <f>SUM(E21,G21,I21,K21,M21,O21)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E21">
@@ -8300,7 +8300,7 @@
         <v>275</v>
       </c>
       <c r="D22">
-        <f>SUM(E22,G22,I22,K22,M22,O22)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E22">
@@ -8327,20 +8327,20 @@
         <v>455</v>
       </c>
       <c r="D23">
-        <f>SUM(E23,G23,I23,K23,M23,O23)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
@@ -8354,7 +8354,7 @@
         <v>471</v>
       </c>
       <c r="D24">
-        <f>SUM(E24,G24,I24,K24,M24,O24)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G24">
@@ -8381,14 +8381,14 @@
         <v>471</v>
       </c>
       <c r="D25">
-        <f>SUM(E25,G25,I25,K25,M25,O25)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -8408,7 +8408,7 @@
         <v>291</v>
       </c>
       <c r="D26">
-        <f>SUM(E26,G26,I26,K26,M26,O26)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G26">
@@ -8432,7 +8432,7 @@
         <v>268</v>
       </c>
       <c r="D27">
-        <f>SUM(E27,G27,I27,K27,M27,O27)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M27">
@@ -8459,7 +8459,7 @@
         <v>268</v>
       </c>
       <c r="D28">
-        <f>SUM(E28,G28,I28,K28,M28,O28)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K28">
@@ -8486,7 +8486,7 @@
         <v>268</v>
       </c>
       <c r="D29">
-        <f>SUM(E29,G29,I29,K29,M29,O29)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E29">
@@ -8513,7 +8513,7 @@
         <v>296</v>
       </c>
       <c r="D30">
-        <f>SUM(E30,G30,I30,K30,M30,O30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G30">
@@ -8534,14 +8534,14 @@
         <v>296</v>
       </c>
       <c r="D31">
-        <f>SUM(E31,G31,I31,K31,M31,O31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
@@ -8555,7 +8555,7 @@
         <v>296</v>
       </c>
       <c r="D32">
-        <f>SUM(E32,G32,I32,K32,M32,O32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K32">
@@ -8576,7 +8576,7 @@
         <v>296</v>
       </c>
       <c r="D33">
-        <f>SUM(E33,G33,I33,K33,M33,O33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O33">
@@ -8597,7 +8597,7 @@
         <v>296</v>
       </c>
       <c r="D34">
-        <f>SUM(E34,G34,I34,K34,M34,O34)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M34">
@@ -8618,7 +8618,7 @@
         <v>296</v>
       </c>
       <c r="D35">
-        <f>SUM(E35,G35,I35,K35,M35,O35)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K35">
@@ -8639,7 +8639,7 @@
         <v>296</v>
       </c>
       <c r="D36">
-        <f>SUM(E36,G36,I36,K36,M36,O36)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M36">
@@ -8660,7 +8660,7 @@
         <v>296</v>
       </c>
       <c r="D37">
-        <f>SUM(E37,G37,I37,K37,M37,O37)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O37">
@@ -8681,7 +8681,7 @@
         <v>296</v>
       </c>
       <c r="D38">
-        <f>SUM(E38,G38,I38,K38,M38,O38)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M38">
@@ -8702,7 +8702,7 @@
         <v>296</v>
       </c>
       <c r="D39">
-        <f>SUM(E39,G39,I39,K39,M39,O39)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K39">
@@ -8723,7 +8723,7 @@
         <v>478</v>
       </c>
       <c r="D40">
-        <f>SUM(E40,G40,I40,K40,M40,O40)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K40">
@@ -8744,7 +8744,7 @@
         <v>478</v>
       </c>
       <c r="D41">
-        <f>SUM(E41,G41,I41,K41,M41,O41)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K41">
@@ -8765,7 +8765,7 @@
         <v>478</v>
       </c>
       <c r="D42">
-        <f>SUM(E42,G42,I42,K42,M42,O42)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K42">
@@ -8786,7 +8786,7 @@
         <v>275</v>
       </c>
       <c r="D43">
-        <f>SUM(E43,G43,I43,K43,M43,O43)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G43">
@@ -8807,7 +8807,7 @@
         <v>275</v>
       </c>
       <c r="D44">
-        <f>SUM(E44,G44,I44,K44,M44,O44)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G44">
@@ -8828,7 +8828,7 @@
         <v>331</v>
       </c>
       <c r="D45">
-        <f>SUM(E45,G45,I45,K45,M45,O45)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H45">
@@ -8852,7 +8852,7 @@
         <v>331</v>
       </c>
       <c r="D46">
-        <f>SUM(E46,G46,I46,K46,M46,O46)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M46">
@@ -8873,7 +8873,7 @@
         <v>275</v>
       </c>
       <c r="D47">
-        <f>SUM(E47,G47,I47,K47,M47,O47)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K47">
@@ -8894,7 +8894,7 @@
         <v>335</v>
       </c>
       <c r="D48">
-        <f>SUM(E48,G48,I48,K48,M48,O48)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K48">
@@ -8915,7 +8915,7 @@
         <v>275</v>
       </c>
       <c r="D49">
-        <f>SUM(E49,G49,I49,K49,M49,O49)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M49">
@@ -8933,7 +8933,7 @@
         <v>331</v>
       </c>
       <c r="D50">
-        <f>SUM(E50,G50,I50,K50,M50,O50)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M50">
@@ -8954,7 +8954,7 @@
         <v>331</v>
       </c>
       <c r="D51">
-        <f>SUM(E51,G51,I51,K51,M51,O51)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M51">
@@ -8975,7 +8975,7 @@
         <v>331</v>
       </c>
       <c r="D52">
-        <f>SUM(E52,G52,I52,K52,M52,O52)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K52">
@@ -8996,7 +8996,7 @@
         <v>335</v>
       </c>
       <c r="D53">
-        <f>SUM(E53,G53,I53,K53,M53,O53)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M53">
@@ -9017,7 +9017,7 @@
         <v>335</v>
       </c>
       <c r="D54">
-        <f>SUM(E54,G54,I54,K54,M54,O54)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O54">
@@ -9038,7 +9038,7 @@
         <v>331</v>
       </c>
       <c r="D55">
-        <f>SUM(E55,G55,I55,K55,M55,O55)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O55">
@@ -9059,7 +9059,7 @@
         <v>331</v>
       </c>
       <c r="D56">
-        <f>SUM(E56,G56,I56,K56,M56,O56)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O56">
@@ -9080,14 +9080,14 @@
         <v>329</v>
       </c>
       <c r="D57">
-        <f>SUM(E57,G57,I57,K57,M57,O57)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I57">
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.45">
@@ -9101,7 +9101,7 @@
         <v>329</v>
       </c>
       <c r="D58">
-        <f>SUM(E58,G58,I58,K58,M58,O58)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K58">
@@ -9122,7 +9122,7 @@
         <v>329</v>
       </c>
       <c r="D59">
-        <f>SUM(E59,G59,I59,K59,M59,O59)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K59">
@@ -9143,7 +9143,7 @@
         <v>329</v>
       </c>
       <c r="D60">
-        <f>SUM(E60,G60,I60,K60,M60,O60)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K60">
@@ -9164,7 +9164,7 @@
         <v>243</v>
       </c>
       <c r="D61">
-        <f>SUM(E61,G61,I61,K61,M61,O61)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G61">
@@ -9185,7 +9185,7 @@
         <v>243</v>
       </c>
       <c r="D62">
-        <f>SUM(E62,G62,I62,K62,M62,O62)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G62">
@@ -9206,7 +9206,7 @@
         <v>243</v>
       </c>
       <c r="D63">
-        <f>SUM(E63,G63,I63,K63,M63,O63)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K63">
@@ -9227,14 +9227,14 @@
         <v>241</v>
       </c>
       <c r="D64">
-        <f>SUM(E64,G64,I64,K64,M64,O64)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.45">
@@ -9248,7 +9248,7 @@
         <v>471</v>
       </c>
       <c r="D65">
-        <f>SUM(E65,G65,I65,K65,M65,O65)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K65">
@@ -9269,7 +9269,7 @@
         <v>239</v>
       </c>
       <c r="D66">
-        <f>SUM(E66,G66,I66,K66,M66,O66)</f>
+        <f t="shared" ref="D66:D129" si="1">SUM(E66,G66,I66,K66,M66,O66)</f>
         <v>1</v>
       </c>
       <c r="G66">
@@ -9290,7 +9290,7 @@
         <v>471</v>
       </c>
       <c r="D67">
-        <f>SUM(E67,G67,I67,K67,M67,O67)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K67">
@@ -9311,7 +9311,7 @@
         <v>240</v>
       </c>
       <c r="D68">
-        <f>SUM(E68,G68,I68,K68,M68,O68)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G68">
@@ -9332,7 +9332,7 @@
         <v>471</v>
       </c>
       <c r="D69">
-        <f>SUM(E69,G69,I69,K69,M69,O69)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K69">
@@ -9353,7 +9353,7 @@
         <v>471</v>
       </c>
       <c r="D70">
-        <f>SUM(E70,G70,I70,K70,M70,O70)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K70">
@@ -9374,7 +9374,7 @@
         <v>287</v>
       </c>
       <c r="D71">
-        <f>SUM(E71,G71,I71,K71,M71,O71)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G71">
@@ -9395,7 +9395,7 @@
         <v>311</v>
       </c>
       <c r="D72">
-        <f>SUM(E72,G72,I72,K72,M72,O72)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K72">
@@ -9416,7 +9416,7 @@
         <v>268</v>
       </c>
       <c r="D73">
-        <f>SUM(E73,G73,I73,K73,M73,O73)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O73">
@@ -9437,7 +9437,7 @@
         <v>311</v>
       </c>
       <c r="D74">
-        <f>SUM(E74,G74,I74,K74,M74,O74)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K74">
@@ -9458,7 +9458,7 @@
         <v>268</v>
       </c>
       <c r="D75">
-        <f>SUM(E75,G75,I75,K75,M75,O75)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K75">
@@ -9479,7 +9479,7 @@
         <v>311</v>
       </c>
       <c r="D76">
-        <f>SUM(E76,G76,I76,K76,M76,O76)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K76">
@@ -9500,7 +9500,7 @@
         <v>287</v>
       </c>
       <c r="D77">
-        <f>SUM(E77,G77,I77,K77,M77,O77)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K77">
@@ -9521,7 +9521,7 @@
         <v>311</v>
       </c>
       <c r="D78">
-        <f>SUM(E78,G78,I78,K78,M78,O78)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K78">
@@ -9542,7 +9542,7 @@
         <v>268</v>
       </c>
       <c r="D79">
-        <f>SUM(E79,G79,I79,K79,M79,O79)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K79">
@@ -9563,7 +9563,7 @@
         <v>311</v>
       </c>
       <c r="D80">
-        <f>SUM(E80,G80,I80,K80,M80,O80)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K80">
@@ -9584,7 +9584,7 @@
         <v>311</v>
       </c>
       <c r="D81">
-        <f>SUM(E81,G81,I81,K81,M81,O81)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M81">
@@ -9605,7 +9605,7 @@
         <v>311</v>
       </c>
       <c r="D82">
-        <f>SUM(E82,G82,I82,K82,M82,O82)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M82">
@@ -9626,7 +9626,7 @@
         <v>291</v>
       </c>
       <c r="D83">
-        <f>SUM(E83,G83,I83,K83,M83,O83)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K83">
@@ -9647,7 +9647,7 @@
         <v>287</v>
       </c>
       <c r="D84">
-        <f>SUM(E84,G84,I84,K84,M84,O84)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E84">
@@ -9668,7 +9668,7 @@
         <v>311</v>
       </c>
       <c r="D85">
-        <f>SUM(E85,G85,I85,K85,M85,O85)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K85">
@@ -9689,7 +9689,7 @@
         <v>268</v>
       </c>
       <c r="D86">
-        <f>SUM(E86,G86,I86,K86,M86,O86)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K86">
@@ -9710,7 +9710,7 @@
         <v>311</v>
       </c>
       <c r="D87">
-        <f>SUM(E87,G87,I87,K87,M87,O87)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K87">
@@ -9731,7 +9731,7 @@
         <v>287</v>
       </c>
       <c r="D88">
-        <f>SUM(E88,G88,I88,K88,M88,O88)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E88">
@@ -9752,7 +9752,7 @@
         <v>311</v>
       </c>
       <c r="D89">
-        <f>SUM(E89,G89,I89,K89,M89,O89)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M89">
@@ -9773,7 +9773,7 @@
         <v>311</v>
       </c>
       <c r="D90">
-        <f>SUM(E90,G90,I90,K90,M90,O90)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M90">
@@ -9794,7 +9794,7 @@
         <v>311</v>
       </c>
       <c r="D91">
-        <f>SUM(E91,G91,I91,K91,M91,O91)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M91">
@@ -9815,7 +9815,7 @@
         <v>268</v>
       </c>
       <c r="D92">
-        <f>SUM(E92,G92,I92,K92,M92,O92)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K92">
@@ -9836,7 +9836,7 @@
         <v>268</v>
       </c>
       <c r="D93">
-        <f>SUM(E93,G93,I93,K93,M93,O93)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K93">
@@ -9857,7 +9857,7 @@
         <v>311</v>
       </c>
       <c r="D94">
-        <f>SUM(E94,G94,I94,K94,M94,O94)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M94">
@@ -9878,7 +9878,7 @@
         <v>311</v>
       </c>
       <c r="D95">
-        <f>SUM(E95,G95,I95,K95,M95,O95)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K95">
@@ -9899,7 +9899,7 @@
         <v>287</v>
       </c>
       <c r="D96">
-        <f>SUM(E96,G96,I96,K96,M96,O96)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K96">
@@ -9920,7 +9920,7 @@
         <v>311</v>
       </c>
       <c r="D97">
-        <f>SUM(E97,G97,I97,K97,M97,O97)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K97">
@@ -9941,7 +9941,7 @@
         <v>296</v>
       </c>
       <c r="D98">
-        <f>SUM(E98,G98,I98,K98,M98,O98)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E98">
@@ -9992,7 +9992,7 @@
         <v>296</v>
       </c>
       <c r="D99">
-        <f>SUM(E99,G99,I99,K99,M99,O99)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E99">
@@ -10043,7 +10043,7 @@
         <v>296</v>
       </c>
       <c r="D100">
-        <f>SUM(E100,G100,I100,K100,M100,O100)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E100">
@@ -10094,7 +10094,7 @@
         <v>296</v>
       </c>
       <c r="D101">
-        <f>SUM(E101,G101,I101,K101,M101,O101)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10109,7 +10109,7 @@
         <v>296</v>
       </c>
       <c r="D102">
-        <f>SUM(E102,G102,I102,K102,M102,O102)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10124,7 +10124,7 @@
         <v>296</v>
       </c>
       <c r="D103">
-        <f>SUM(E103,G103,I103,K103,M103,O103)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10139,7 +10139,7 @@
         <v>296</v>
       </c>
       <c r="D104">
-        <f>SUM(E104,G104,I104,K104,M104,O104)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10154,7 +10154,7 @@
         <v>296</v>
       </c>
       <c r="D105">
-        <f>SUM(E105,G105,I105,K105,M105,O105)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10169,7 +10169,7 @@
         <v>296</v>
       </c>
       <c r="D106">
-        <f>SUM(E106,G106,I106,K106,M106,O106)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10184,7 +10184,7 @@
         <v>296</v>
       </c>
       <c r="D107">
-        <f>SUM(E107,G107,I107,K107,M107,O107)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10199,7 +10199,7 @@
         <v>296</v>
       </c>
       <c r="D108">
-        <f>SUM(E108,G108,I108,K108,M108,O108)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10214,7 +10214,7 @@
         <v>478</v>
       </c>
       <c r="D109">
-        <f>SUM(E109,G109,I109,K109,M109,O109)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E109">
@@ -10265,7 +10265,7 @@
         <v>331</v>
       </c>
       <c r="D110">
-        <f>SUM(E110,G110,I110,K110,M110,O110)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10280,7 +10280,7 @@
         <v>335</v>
       </c>
       <c r="D111">
-        <f>SUM(E111,G111,I111,K111,M111,O111)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10295,7 +10295,7 @@
         <v>275</v>
       </c>
       <c r="D112">
-        <f>SUM(E112,G112,I112,K112,M112,O112)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10310,7 +10310,7 @@
         <v>331</v>
       </c>
       <c r="D113">
-        <f>SUM(E113,G113,I113,K113,M113,O113)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10325,7 +10325,7 @@
         <v>335</v>
       </c>
       <c r="D114">
-        <f>SUM(E114,G114,I114,K114,M114,O114)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10340,7 +10340,7 @@
         <v>335</v>
       </c>
       <c r="D115">
-        <f>SUM(E115,G115,I115,K115,M115,O115)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10355,7 +10355,7 @@
         <v>331</v>
       </c>
       <c r="D116">
-        <f>SUM(E116,G116,I116,K116,M116,O116)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10370,7 +10370,7 @@
         <v>331</v>
       </c>
       <c r="D117">
-        <f>SUM(E117,G117,I117,K117,M117,O117)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10385,7 +10385,7 @@
         <v>335</v>
       </c>
       <c r="D118">
-        <f>SUM(E118,G118,I118,K118,M118,O118)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10400,7 +10400,7 @@
         <v>335</v>
       </c>
       <c r="D119">
-        <f>SUM(E119,G119,I119,K119,M119,O119)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10415,7 +10415,7 @@
         <v>335</v>
       </c>
       <c r="D120">
-        <f>SUM(E120,G120,I120,K120,M120,O120)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10430,7 +10430,7 @@
         <v>335</v>
       </c>
       <c r="D121">
-        <f>SUM(E121,G121,I121,K121,M121,O121)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10445,7 +10445,7 @@
         <v>335</v>
       </c>
       <c r="D122">
-        <f>SUM(E122,G122,I122,K122,M122,O122)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10460,7 +10460,7 @@
         <v>335</v>
       </c>
       <c r="D123">
-        <f>SUM(E123,G123,I123,K123,M123,O123)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10475,7 +10475,7 @@
         <v>335</v>
       </c>
       <c r="D124">
-        <f>SUM(E124,G124,I124,K124,M124,O124)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10490,7 +10490,7 @@
         <v>331</v>
       </c>
       <c r="D125">
-        <f>SUM(E125,G125,I125,K125,M125,O125)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10505,7 +10505,7 @@
         <v>275</v>
       </c>
       <c r="D126">
-        <f>SUM(E126,G126,I126,K126,M126,O126)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10520,7 +10520,7 @@
         <v>275</v>
       </c>
       <c r="D127">
-        <f>SUM(E127,G127,I127,K127,M127,O127)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10535,7 +10535,7 @@
         <v>331</v>
       </c>
       <c r="D128">
-        <f>SUM(E128,G128,I128,K128,M128,O128)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10550,7 +10550,7 @@
         <v>275</v>
       </c>
       <c r="D129">
-        <f>SUM(E129,G129,I129,K129,M129,O129)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -10565,7 +10565,7 @@
         <v>335</v>
       </c>
       <c r="D130">
-        <f>SUM(E130,G130,I130,K130,M130,O130)</f>
+        <f t="shared" ref="D130:D193" si="2">SUM(E130,G130,I130,K130,M130,O130)</f>
         <v>0</v>
       </c>
     </row>
@@ -10580,7 +10580,7 @@
         <v>335</v>
       </c>
       <c r="D131">
-        <f>SUM(E131,G131,I131,K131,M131,O131)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10595,7 +10595,7 @@
         <v>331</v>
       </c>
       <c r="D132">
-        <f>SUM(E132,G132,I132,K132,M132,O132)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10610,7 +10610,7 @@
         <v>331</v>
       </c>
       <c r="D133">
-        <f>SUM(E133,G133,I133,K133,M133,O133)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10625,7 +10625,7 @@
         <v>331</v>
       </c>
       <c r="D134">
-        <f>SUM(E134,G134,I134,K134,M134,O134)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10640,7 +10640,7 @@
         <v>335</v>
       </c>
       <c r="D135">
-        <f>SUM(E135,G135,I135,K135,M135,O135)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10655,7 +10655,7 @@
         <v>331</v>
       </c>
       <c r="D136">
-        <f>SUM(E136,G136,I136,K136,M136,O136)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10670,7 +10670,7 @@
         <v>331</v>
       </c>
       <c r="D137">
-        <f>SUM(E137,G137,I137,K137,M137,O137)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10685,7 +10685,7 @@
         <v>275</v>
       </c>
       <c r="D138">
-        <f>SUM(E138,G138,I138,K138,M138,O138)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10700,7 +10700,7 @@
         <v>335</v>
       </c>
       <c r="D139">
-        <f>SUM(E139,G139,I139,K139,M139,O139)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10715,7 +10715,7 @@
         <v>331</v>
       </c>
       <c r="D140">
-        <f>SUM(E140,G140,I140,K140,M140,O140)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10730,7 +10730,7 @@
         <v>335</v>
       </c>
       <c r="D141">
-        <f>SUM(E141,G141,I141,K141,M141,O141)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10745,7 +10745,7 @@
         <v>331</v>
       </c>
       <c r="D142">
-        <f>SUM(E142,G142,I142,K142,M142,O142)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10760,7 +10760,7 @@
         <v>331</v>
       </c>
       <c r="D143">
-        <f>SUM(E143,G143,I143,K143,M143,O143)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10775,7 +10775,7 @@
         <v>331</v>
       </c>
       <c r="D144">
-        <f>SUM(E144,G144,I144,K144,M144,O144)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10790,7 +10790,7 @@
         <v>275</v>
       </c>
       <c r="D145">
-        <f>SUM(E145,G145,I145,K145,M145,O145)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10805,7 +10805,7 @@
         <v>275</v>
       </c>
       <c r="D146">
-        <f>SUM(E146,G146,I146,K146,M146,O146)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10820,7 +10820,7 @@
         <v>335</v>
       </c>
       <c r="D147">
-        <f>SUM(E147,G147,I147,K147,M147,O147)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10835,7 +10835,7 @@
         <v>335</v>
       </c>
       <c r="D148">
-        <f>SUM(E148,G148,I148,K148,M148,O148)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10850,7 +10850,7 @@
         <v>335</v>
       </c>
       <c r="D149">
-        <f>SUM(E149,G149,I149,K149,M149,O149)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10865,7 +10865,7 @@
         <v>331</v>
       </c>
       <c r="D150">
-        <f>SUM(E150,G150,I150,K150,M150,O150)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10880,7 +10880,7 @@
         <v>331</v>
       </c>
       <c r="D151">
-        <f>SUM(E151,G151,I151,K151,M151,O151)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10895,7 +10895,7 @@
         <v>335</v>
       </c>
       <c r="D152">
-        <f>SUM(E152,G152,I152,K152,M152,O152)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10910,7 +10910,7 @@
         <v>335</v>
       </c>
       <c r="D153">
-        <f>SUM(E153,G153,I153,K153,M153,O153)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10925,7 +10925,7 @@
         <v>275</v>
       </c>
       <c r="D154">
-        <f>SUM(E154,G154,I154,K154,M154,O154)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10940,7 +10940,7 @@
         <v>335</v>
       </c>
       <c r="D155">
-        <f>SUM(E155,G155,I155,K155,M155,O155)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10955,7 +10955,7 @@
         <v>331</v>
       </c>
       <c r="D156">
-        <f>SUM(E156,G156,I156,K156,M156,O156)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10970,7 +10970,7 @@
         <v>335</v>
       </c>
       <c r="D157">
-        <f>SUM(E157,G157,I157,K157,M157,O157)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -10985,7 +10985,7 @@
         <v>329</v>
       </c>
       <c r="D158">
-        <f>SUM(E158,G158,I158,K158,M158,O158)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11000,7 +11000,7 @@
         <v>455</v>
       </c>
       <c r="D159">
-        <f>SUM(E159,G159,I159,K159,M159,O159)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11015,7 +11015,7 @@
         <v>238</v>
       </c>
       <c r="D160">
-        <f>SUM(E160,G160,I160,K160,M160,O160)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11030,7 +11030,7 @@
         <v>238</v>
       </c>
       <c r="D161">
-        <f>SUM(E161,G161,I161,K161,M161,O161)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11045,7 +11045,7 @@
         <v>237</v>
       </c>
       <c r="D162">
-        <f>SUM(E162,G162,I162,K162,M162,O162)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11060,7 +11060,7 @@
         <v>455</v>
       </c>
       <c r="D163">
-        <f>SUM(E163,G163,I163,K163,M163,O163)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11075,7 +11075,7 @@
         <v>329</v>
       </c>
       <c r="D164">
-        <f>SUM(E164,G164,I164,K164,M164,O164)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11090,7 +11090,7 @@
         <v>329</v>
       </c>
       <c r="D165">
-        <f>SUM(E165,G165,I165,K165,M165,O165)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11105,7 +11105,7 @@
         <v>237</v>
       </c>
       <c r="D166">
-        <f>SUM(E166,G166,I166,K166,M166,O166)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11120,7 +11120,7 @@
         <v>238</v>
       </c>
       <c r="D167">
-        <f>SUM(E167,G167,I167,K167,M167,O167)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11135,7 +11135,7 @@
         <v>237</v>
       </c>
       <c r="D168">
-        <f>SUM(E168,G168,I168,K168,M168,O168)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11150,7 +11150,7 @@
         <v>329</v>
       </c>
       <c r="D169">
-        <f>SUM(E169,G169,I169,K169,M169,O169)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11165,7 +11165,7 @@
         <v>237</v>
       </c>
       <c r="D170">
-        <f>SUM(E170,G170,I170,K170,M170,O170)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11180,7 +11180,7 @@
         <v>238</v>
       </c>
       <c r="D171">
-        <f>SUM(E171,G171,I171,K171,M171,O171)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11195,7 +11195,7 @@
         <v>329</v>
       </c>
       <c r="D172">
-        <f>SUM(E172,G172,I172,K172,M172,O172)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11210,7 +11210,7 @@
         <v>237</v>
       </c>
       <c r="D173">
-        <f>SUM(E173,G173,I173,K173,M173,O173)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11225,7 +11225,7 @@
         <v>455</v>
       </c>
       <c r="D174">
-        <f>SUM(E174,G174,I174,K174,M174,O174)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11240,7 +11240,7 @@
         <v>329</v>
       </c>
       <c r="D175">
-        <f>SUM(E175,G175,I175,K175,M175,O175)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11255,7 +11255,7 @@
         <v>455</v>
       </c>
       <c r="D176">
-        <f>SUM(E176,G176,I176,K176,M176,O176)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11270,7 +11270,7 @@
         <v>455</v>
       </c>
       <c r="D177">
-        <f>SUM(E177,G177,I177,K177,M177,O177)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11285,7 +11285,7 @@
         <v>455</v>
       </c>
       <c r="D178">
-        <f>SUM(E178,G178,I178,K178,M178,O178)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11300,7 +11300,7 @@
         <v>329</v>
       </c>
       <c r="D179">
-        <f>SUM(E179,G179,I179,K179,M179,O179)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11315,7 +11315,7 @@
         <v>455</v>
       </c>
       <c r="D180">
-        <f>SUM(E180,G180,I180,K180,M180,O180)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11330,7 +11330,7 @@
         <v>455</v>
       </c>
       <c r="D181">
-        <f>SUM(E181,G181,I181,K181,M181,O181)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11345,7 +11345,7 @@
         <v>329</v>
       </c>
       <c r="D182">
-        <f>SUM(E182,G182,I182,K182,M182,O182)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11360,7 +11360,7 @@
         <v>238</v>
       </c>
       <c r="D183">
-        <f>SUM(E183,G183,I183,K183,M183,O183)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11375,7 +11375,7 @@
         <v>238</v>
       </c>
       <c r="D184">
-        <f>SUM(E184,G184,I184,K184,M184,O184)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11390,7 +11390,7 @@
         <v>237</v>
       </c>
       <c r="D185">
-        <f>SUM(E185,G185,I185,K185,M185,O185)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11405,7 +11405,7 @@
         <v>455</v>
       </c>
       <c r="D186">
-        <f>SUM(E186,G186,I186,K186,M186,O186)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11420,7 +11420,7 @@
         <v>329</v>
       </c>
       <c r="D187">
-        <f>SUM(E187,G187,I187,K187,M187,O187)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11435,7 +11435,7 @@
         <v>329</v>
       </c>
       <c r="D188">
-        <f>SUM(E188,G188,I188,K188,M188,O188)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11450,7 +11450,7 @@
         <v>455</v>
       </c>
       <c r="D189">
-        <f>SUM(E189,G189,I189,K189,M189,O189)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11465,7 +11465,7 @@
         <v>455</v>
       </c>
       <c r="D190">
-        <f>SUM(E190,G190,I190,K190,M190,O190)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11480,7 +11480,7 @@
         <v>245</v>
       </c>
       <c r="D191">
-        <f>SUM(E191,G191,I191,K191,M191,O191)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11495,7 +11495,7 @@
         <v>243</v>
       </c>
       <c r="D192">
-        <f>SUM(E192,G192,I192,K192,M192,O192)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11510,7 +11510,7 @@
         <v>243</v>
       </c>
       <c r="D193">
-        <f>SUM(E193,G193,I193,K193,M193,O193)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11525,7 +11525,7 @@
         <v>243</v>
       </c>
       <c r="D194">
-        <f>SUM(E194,G194,I194,K194,M194,O194)</f>
+        <f t="shared" ref="D194:D257" si="3">SUM(E194,G194,I194,K194,M194,O194)</f>
         <v>0</v>
       </c>
     </row>
@@ -11540,7 +11540,7 @@
         <v>243</v>
       </c>
       <c r="D195">
-        <f>SUM(E195,G195,I195,K195,M195,O195)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11555,7 +11555,7 @@
         <v>243</v>
       </c>
       <c r="D196">
-        <f>SUM(E196,G196,I196,K196,M196,O196)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11570,7 +11570,7 @@
         <v>243</v>
       </c>
       <c r="D197">
-        <f>SUM(E197,G197,I197,K197,M197,O197)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11585,7 +11585,7 @@
         <v>243</v>
       </c>
       <c r="D198">
-        <f>SUM(E198,G198,I198,K198,M198,O198)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11600,7 +11600,7 @@
         <v>243</v>
       </c>
       <c r="D199">
-        <f>SUM(E199,G199,I199,K199,M199,O199)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11615,7 +11615,7 @@
         <v>243</v>
       </c>
       <c r="D200">
-        <f>SUM(E200,G200,I200,K200,M200,O200)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11630,7 +11630,7 @@
         <v>243</v>
       </c>
       <c r="D201">
-        <f>SUM(E201,G201,I201,K201,M201,O201)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11645,7 +11645,7 @@
         <v>243</v>
       </c>
       <c r="D202">
-        <f>SUM(E202,G202,I202,K202,M202,O202)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11660,7 +11660,7 @@
         <v>243</v>
       </c>
       <c r="D203">
-        <f>SUM(E203,G203,I203,K203,M203,O203)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11675,7 +11675,7 @@
         <v>243</v>
       </c>
       <c r="D204">
-        <f>SUM(E204,G204,I204,K204,M204,O204)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11690,7 +11690,7 @@
         <v>243</v>
       </c>
       <c r="D205">
-        <f>SUM(E205,G205,I205,K205,M205,O205)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11705,7 +11705,7 @@
         <v>243</v>
       </c>
       <c r="D206">
-        <f>SUM(E206,G206,I206,K206,M206,O206)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11720,7 +11720,7 @@
         <v>242</v>
       </c>
       <c r="D207">
-        <f>SUM(E207,G207,I207,K207,M207,O207)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E207">
@@ -11771,7 +11771,7 @@
         <v>242</v>
       </c>
       <c r="D208">
-        <f>SUM(E208,G208,I208,K208,M208,O208)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E208">
@@ -11822,7 +11822,7 @@
         <v>242</v>
       </c>
       <c r="D209">
-        <f>SUM(E209,G209,I209,K209,M209,O209)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E209">
@@ -11873,7 +11873,7 @@
         <v>243</v>
       </c>
       <c r="D210">
-        <f>SUM(E210,G210,I210,K210,M210,O210)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11888,7 +11888,7 @@
         <v>243</v>
       </c>
       <c r="D211">
-        <f>SUM(E211,G211,I211,K211,M211,O211)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11903,7 +11903,7 @@
         <v>243</v>
       </c>
       <c r="D212">
-        <f>SUM(E212,G212,I212,K212,M212,O212)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11918,7 +11918,7 @@
         <v>268</v>
       </c>
       <c r="D213">
-        <f>SUM(E213,G213,I213,K213,M213,O213)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E213">
@@ -11969,7 +11969,7 @@
         <v>268</v>
       </c>
       <c r="D214">
-        <f>SUM(E214,G214,I214,K214,M214,O214)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11984,7 +11984,7 @@
         <v>268</v>
       </c>
       <c r="D215">
-        <f>SUM(E215,G215,I215,K215,M215,O215)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -11999,7 +11999,7 @@
         <v>268</v>
       </c>
       <c r="D216">
-        <f>SUM(E216,G216,I216,K216,M216,O216)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12014,7 +12014,7 @@
         <v>311</v>
       </c>
       <c r="D217">
-        <f>SUM(E217,G217,I217,K217,M217,O217)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12029,7 +12029,7 @@
         <v>268</v>
       </c>
       <c r="D218">
-        <f>SUM(E218,G218,I218,K218,M218,O218)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12044,7 +12044,7 @@
         <v>268</v>
       </c>
       <c r="D219">
-        <f>SUM(E219,G219,I219,K219,M219,O219)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12059,7 +12059,7 @@
         <v>267</v>
       </c>
       <c r="D220">
-        <f>SUM(E220,G220,I220,K220,M220,O220)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12074,7 +12074,7 @@
         <v>268</v>
       </c>
       <c r="D221">
-        <f>SUM(E221,G221,I221,K221,M221,O221)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12089,7 +12089,7 @@
         <v>311</v>
       </c>
       <c r="D222">
-        <f>SUM(E222,G222,I222,K222,M222,O222)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12104,7 +12104,7 @@
         <v>267</v>
       </c>
       <c r="D223">
-        <f>SUM(E223,G223,I223,K223,M223,O223)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12119,7 +12119,7 @@
         <v>311</v>
       </c>
       <c r="D224">
-        <f>SUM(E224,G224,I224,K224,M224,O224)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12134,7 +12134,7 @@
         <v>268</v>
       </c>
       <c r="D225">
-        <f>SUM(E225,G225,I225,K225,M225,O225)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12149,7 +12149,7 @@
         <v>291</v>
       </c>
       <c r="D226">
-        <f>SUM(E226,G226,I226,K226,M226,O226)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12164,7 +12164,7 @@
         <v>291</v>
       </c>
       <c r="D227">
-        <f>SUM(E227,G227,I227,K227,M227,O227)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12179,7 +12179,7 @@
         <v>291</v>
       </c>
       <c r="D228">
-        <f>SUM(E228,G228,I228,K228,M228,O228)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12194,7 +12194,7 @@
         <v>268</v>
       </c>
       <c r="D229">
-        <f>SUM(E229,G229,I229,K229,M229,O229)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12209,7 +12209,7 @@
         <v>268</v>
       </c>
       <c r="D230">
-        <f>SUM(E230,G230,I230,K230,M230,O230)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12224,7 +12224,7 @@
         <v>268</v>
       </c>
       <c r="D231">
-        <f>SUM(E231,G231,I231,K231,M231,O231)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12239,7 +12239,7 @@
         <v>268</v>
       </c>
       <c r="D232">
-        <f>SUM(E232,G232,I232,K232,M232,O232)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12254,7 +12254,7 @@
         <v>268</v>
       </c>
       <c r="D233">
-        <f>SUM(E233,G233,I233,K233,M233,O233)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12269,7 +12269,7 @@
         <v>267</v>
       </c>
       <c r="D234">
-        <f>SUM(E234,G234,I234,K234,M234,O234)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12284,7 +12284,7 @@
         <v>268</v>
       </c>
       <c r="D235">
-        <f>SUM(E235,G235,I235,K235,M235,O235)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12299,7 +12299,7 @@
         <v>268</v>
       </c>
       <c r="D236">
-        <f>SUM(E236,G236,I236,K236,M236,O236)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>